<commit_message>
small input data update and changed name of the cli function
</commit_message>
<xml_diff>
--- a/examples/inputs/MGM_hourly/MGM_Test-Saatlik Güneşlenme Süresi (saat).xlsx
+++ b/examples/inputs/MGM_hourly/MGM_Test-Saatlik Güneşlenme Süresi (saat).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\PyPrecip\examples\inputs\MGM_hourly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5987C36B-36F9-485D-A52C-40DD95F524A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C4BF51-38BC-4A58-A395-4106F0E1F5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46800" yWindow="7635" windowWidth="18885" windowHeight="15585" xr2:uid="{BFA45771-B0DE-4F15-8068-1A40B5FA437A}"/>
+    <workbookView xWindow="1193" yWindow="1508" windowWidth="21600" windowHeight="11054" xr2:uid="{BFA45771-B0DE-4F15-8068-1A40B5FA437A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="44">
   <si>
     <t>T.C. 
 ÇEVRE,ŞEHİRCİLİK VE İKLİM DEĞİŞİKLİĞİ BAKANLIĞI 
@@ -168,12 +168,15 @@
   <si>
     <t>Yıl/Ay: 2024/5  İstasyon Adı/No: DOĞANYOL/18352</t>
   </si>
+  <si>
+    <t>0.10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +218,13 @@
       <color rgb="FF000000"/>
       <name val="SansSerif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -743,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87DF27B-B222-4D45-BA8C-7944D6221EB2}">
   <dimension ref="A2:AC157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92:X92"/>
+    <sheetView tabSelected="1" topLeftCell="C92" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P114" sqref="P114:W114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -962,28 +972,28 @@
         <v>28</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>30</v>
@@ -995,22 +1005,22 @@
         <v>30</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>28</v>
@@ -1041,28 +1051,28 @@
         <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>30</v>
@@ -1120,28 +1130,28 @@
         <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>30</v>
@@ -1202,49 +1212,49 @@
         <v>30</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U10" s="5" t="s">
         <v>30</v>
@@ -1284,28 +1294,28 @@
         <v>30</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>30</v>
@@ -1366,28 +1376,28 @@
         <v>30</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>30</v>
@@ -1448,28 +1458,28 @@
         <v>30</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>30</v>
@@ -1530,28 +1540,28 @@
         <v>30</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>30</v>
@@ -2223,22 +2233,54 @@
         <v>28</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="5">
+        <v>1</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5" t="s">
@@ -2379,22 +2421,22 @@
         <v>30</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="U25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V25" s="5" t="s">
         <v>28</v>
@@ -3581,31 +3623,31 @@
         <v>28</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J46" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N46" s="5" t="s">
         <v>30</v>
@@ -3660,31 +3702,31 @@
         <v>28</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I47" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J47" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N47" s="5" t="s">
         <v>30</v>
@@ -3739,31 +3781,31 @@
         <v>28</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F48" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J48" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N48" s="5" t="s">
         <v>30</v>
@@ -3818,34 +3860,34 @@
         <v>28</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F49" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J49" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="K49" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O49" s="5" t="s">
         <v>30</v>
@@ -3897,34 +3939,34 @@
         <v>28</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="K50" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="L50" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O50" s="5" t="s">
         <v>40</v>
@@ -3976,52 +4018,52 @@
         <v>28</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K51" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="L51" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O51" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q51" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R51" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="S51" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U51" s="5" t="s">
         <v>35</v>
@@ -4052,22 +4094,54 @@
         <v>28</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="U52" s="5"/>
       <c r="V52" s="5"/>
       <c r="W52" s="5" t="s">
@@ -4093,22 +4167,54 @@
         <v>28</v>
       </c>
       <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S53" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T53" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="5" t="s">
@@ -4134,22 +4240,54 @@
         <v>28</v>
       </c>
       <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5"/>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R54" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S54" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T54" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="U54" s="5"/>
       <c r="V54" s="5"/>
       <c r="W54" s="5" t="s">
@@ -4175,22 +4313,54 @@
         <v>28</v>
       </c>
       <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="5"/>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5"/>
-      <c r="T55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T55" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="U55" s="5"/>
       <c r="V55" s="5"/>
       <c r="W55" s="5" t="s">
@@ -4216,22 +4386,54 @@
         <v>28</v>
       </c>
       <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="5"/>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S56" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T56" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="U56" s="5"/>
       <c r="V56" s="5"/>
       <c r="W56" s="5" t="s">
@@ -4260,10 +4462,10 @@
         <v>28</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>30</v>
@@ -4290,22 +4492,22 @@
         <v>30</v>
       </c>
       <c r="O57" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="P57" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q57" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R57" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="S57" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U57" s="5" t="s">
         <v>35</v>
@@ -4339,10 +4541,10 @@
         <v>28</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>30</v>
@@ -4360,31 +4562,31 @@
         <v>30</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="Q58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="R58" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="S58" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U58" s="5" t="s">
         <v>35</v>
@@ -4418,13 +4620,13 @@
         <v>28</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>30</v>
@@ -4439,7 +4641,7 @@
         <v>30</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M59" s="5" t="s">
         <v>30</v>
@@ -4454,16 +4656,16 @@
         <v>30</v>
       </c>
       <c r="Q59" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R59" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S59" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T59" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U59" s="5" t="s">
         <v>35</v>
@@ -4503,19 +4705,19 @@
         <v>35</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L60" s="5" t="s">
         <v>30</v>
@@ -4536,13 +4738,13 @@
         <v>30</v>
       </c>
       <c r="R60" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S60" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T60" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U60" s="5" t="s">
         <v>35</v>
@@ -4579,10 +4781,10 @@
         <v>35</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>30</v>
@@ -4615,13 +4817,13 @@
         <v>30</v>
       </c>
       <c r="R61" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S61" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U61" s="5" t="s">
         <v>35</v>
@@ -4655,52 +4857,52 @@
         <v>28</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M62" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N62" s="5" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="N62" s="5">
+        <v>1</v>
       </c>
       <c r="O62" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P62" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q62" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="R62" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S62" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T62" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U62" s="5" t="s">
         <v>35</v>
@@ -4743,10 +4945,10 @@
         <v>35</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>30</v>
@@ -4761,25 +4963,25 @@
         <v>30</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q63" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="R63" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S63" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T63" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U63" s="5" t="s">
         <v>35</v>
@@ -4816,43 +5018,43 @@
         <v>35</v>
       </c>
       <c r="F64" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O64" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P64" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q64" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q64" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="R64" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S64" s="5" t="s">
         <v>35</v>
@@ -4895,43 +5097,43 @@
         <v>35</v>
       </c>
       <c r="F65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N65" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O65" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N65" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O65" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="P65" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q65" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S65" s="5" t="s">
         <v>35</v>
@@ -4974,13 +5176,13 @@
         <v>35</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>30</v>
@@ -4995,10 +5197,10 @@
         <v>30</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N66" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O66" s="5" t="s">
         <v>30</v>
@@ -5010,7 +5212,7 @@
         <v>30</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S66" s="5" t="s">
         <v>35</v>
@@ -5056,14 +5258,14 @@
         <v>35</v>
       </c>
       <c r="G67" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I67" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H67" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J67" s="5" t="s">
         <v>30</v>
       </c>
@@ -5080,22 +5282,22 @@
         <v>30</v>
       </c>
       <c r="O67" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q67" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="S67" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T67" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="U67" s="5" t="s">
         <v>35</v>
@@ -5132,10 +5334,10 @@
         <v>35</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>30</v>
@@ -5162,13 +5364,13 @@
         <v>30</v>
       </c>
       <c r="P68" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q68" s="5" t="s">
         <v>30</v>
       </c>
       <c r="R68" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S68" s="5" t="s">
         <v>35</v>
@@ -5211,10 +5413,10 @@
         <v>35</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>30</v>
@@ -5238,22 +5440,22 @@
         <v>30</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q69" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R69" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S69" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T69" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="R69" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T69" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="U69" s="5" t="s">
         <v>35</v>
@@ -5293,7 +5495,7 @@
         <v>35</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>30</v>
@@ -5320,13 +5522,13 @@
         <v>30</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Q70" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S70" s="5" t="s">
         <v>35</v>
@@ -5369,13 +5571,13 @@
         <v>35</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>30</v>
@@ -5399,13 +5601,13 @@
         <v>30</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="Q71" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S71" s="5" t="s">
         <v>35</v>
@@ -5448,10 +5650,10 @@
         <v>35</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>30</v>
@@ -5475,16 +5677,16 @@
         <v>30</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q72" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S72" s="5" t="s">
         <v>35</v>
@@ -5527,10 +5729,10 @@
         <v>35</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>30</v>
@@ -5554,16 +5756,16 @@
         <v>30</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P73" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q73" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S73" s="5" t="s">
         <v>35</v>
@@ -5606,13 +5808,13 @@
         <v>35</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>30</v>
@@ -5633,16 +5835,16 @@
         <v>30</v>
       </c>
       <c r="O74" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R74" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S74" s="5" t="s">
         <v>35</v>
@@ -6041,28 +6243,28 @@
         <v>28</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L85" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N85" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O85" s="5" t="s">
         <v>30</v>
@@ -6120,52 +6322,52 @@
         <v>28</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>33</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N86" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O86" s="5" t="s">
         <v>30</v>
       </c>
       <c r="P86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R86" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S86" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q86" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R86" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S86" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="T86" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="U86" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="V86" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="W86" s="5" t="s">
         <v>35</v>
@@ -6199,28 +6401,28 @@
         <v>28</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L87" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O87" s="5" t="s">
         <v>30</v>
@@ -6232,19 +6434,19 @@
         <v>30</v>
       </c>
       <c r="R87" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S87" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T87" s="5" t="s">
         <v>30</v>
       </c>
       <c r="U87" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V87" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W87" s="5" t="s">
         <v>35</v>
@@ -6278,52 +6480,52 @@
         <v>28</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H88" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M88" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I88" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="N88" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O88" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q88" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R88" s="5" t="s">
         <v>30</v>
       </c>
       <c r="S88" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="T88" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U88" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V88" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W88" s="5" t="s">
         <v>35</v>
@@ -6357,52 +6559,52 @@
         <v>28</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J89" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K89" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L89" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M89" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N89" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K89" s="5" t="s">
+      <c r="O89" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P89" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q89" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R89" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S89" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R89" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S89" s="5" t="s">
+      <c r="T89" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U89" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V89" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="T89" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U89" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="V89" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="W89" s="5" t="s">
         <v>35</v>
@@ -6436,52 +6638,52 @@
         <v>28</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K90" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L90" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M90" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O90" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I90" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L90" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M90" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N90" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O90" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="P90" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q90" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R90" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S90" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T90" s="5" t="s">
         <v>30</v>
       </c>
       <c r="U90" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="V90" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W90" s="5" t="s">
         <v>35</v>
@@ -6515,7 +6717,7 @@
         <v>28</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>30</v>
@@ -6527,25 +6729,25 @@
         <v>30</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M91" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="N91" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P91" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q91" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="R91" s="5" t="s">
         <v>30</v>
@@ -6557,10 +6759,10 @@
         <v>30</v>
       </c>
       <c r="U91" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="V91" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W91" s="5" t="s">
         <v>35</v>
@@ -6591,22 +6793,54 @@
         <v>28</v>
       </c>
       <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-      <c r="K92" s="5"/>
-      <c r="L92" s="5"/>
-      <c r="M92" s="5"/>
-      <c r="N92" s="5"/>
-      <c r="O92" s="5"/>
-      <c r="P92" s="5"/>
-      <c r="Q92" s="5"/>
-      <c r="R92" s="5"/>
-      <c r="S92" s="5"/>
-      <c r="T92" s="5"/>
-      <c r="U92" s="5"/>
-      <c r="V92" s="5"/>
+      <c r="G92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L92" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O92" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q92" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R92" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U92" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V92" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="W92" s="5"/>
       <c r="X92" s="5"/>
       <c r="Y92" s="5" t="s">
@@ -6635,7 +6869,7 @@
         <v>28</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>30</v>
@@ -6650,37 +6884,37 @@
         <v>30</v>
       </c>
       <c r="L93" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O93" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P93" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N93" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O93" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P93" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="Q93" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="R93" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="S93" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="T93" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U93" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V93" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W93" s="5" t="s">
         <v>35</v>
@@ -6714,28 +6948,28 @@
         <v>28</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N94" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="O94" s="5" t="s">
         <v>30</v>
@@ -6744,22 +6978,22 @@
         <v>30</v>
       </c>
       <c r="Q94" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="R94" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="S94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V94" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W94" s="5" t="s">
         <v>35</v>
@@ -6793,7 +7027,7 @@
         <v>28</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>30</v>
@@ -6811,7 +7045,7 @@
         <v>30</v>
       </c>
       <c r="M95" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="N95" s="5" t="s">
         <v>30</v>
@@ -6835,10 +7069,10 @@
         <v>30</v>
       </c>
       <c r="U95" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="V95" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W95" s="5" t="s">
         <v>35</v>
@@ -6872,7 +7106,7 @@
         <v>28</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H96" s="5" t="s">
         <v>30</v>
@@ -6896,28 +7130,28 @@
         <v>30</v>
       </c>
       <c r="O96" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P96" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q96" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R96" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S96" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="T96" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="U96" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V96" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W96" s="5" t="s">
         <v>35</v>
@@ -6951,13 +7185,13 @@
         <v>28</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J97" s="5" t="s">
         <v>30</v>
@@ -6969,34 +7203,34 @@
         <v>30</v>
       </c>
       <c r="M97" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N97" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R97" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="P97" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q97" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R97" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="S97" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="T97" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U97" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V97" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W97" s="5" t="s">
         <v>35</v>
@@ -7030,10 +7264,10 @@
         <v>28</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>30</v>
@@ -7045,37 +7279,37 @@
         <v>30</v>
       </c>
       <c r="L98" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="M98" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N98" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O98" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="P98" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="Q98" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R98" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="S98" s="5" t="s">
         <v>30</v>
       </c>
       <c r="T98" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="U98" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V98" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W98" s="5" t="s">
         <v>35</v>
@@ -7109,14 +7343,14 @@
         <v>28</v>
       </c>
       <c r="G99" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I99" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H99" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I99" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J99" s="5" t="s">
         <v>30</v>
       </c>
@@ -7127,31 +7361,31 @@
         <v>30</v>
       </c>
       <c r="M99" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="N99" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="O99" s="5" t="s">
         <v>30</v>
       </c>
       <c r="P99" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="Q99" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="R99" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S99" s="5" t="s">
         <v>30</v>
       </c>
       <c r="T99" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U99" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V99" s="5" t="s">
         <v>35</v>
@@ -7188,10 +7422,10 @@
         <v>28</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I100" s="5" t="s">
         <v>30</v>
@@ -7206,25 +7440,25 @@
         <v>30</v>
       </c>
       <c r="M100" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="N100" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="O100" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q100" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R100" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P100" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q100" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R100" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="S100" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="T100" s="5" t="s">
         <v>36</v>
@@ -7267,46 +7501,46 @@
         <v>28</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K101" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L101" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M101" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N101" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O101" s="5">
+        <v>1</v>
+      </c>
+      <c r="P101" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="O101" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P101" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="Q101" s="5" t="s">
         <v>32</v>
       </c>
       <c r="R101" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="S101" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="T101" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="U101" s="5" t="s">
         <v>35</v>
@@ -7349,49 +7583,49 @@
         <v>35</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I102" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P102" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q102" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R102" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J102" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K102" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L102" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M102" s="5" t="s">
+      <c r="S102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T102" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N102" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O102" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P102" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q102" s="5" t="s">
+      <c r="U102" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="R102" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S102" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T102" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U102" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="V102" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W102" s="5" t="s">
         <v>35</v>
@@ -7425,13 +7659,13 @@
         <v>28</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J103" s="5" t="s">
         <v>30</v>
@@ -7443,31 +7677,31 @@
         <v>30</v>
       </c>
       <c r="M103" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="N103" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O103" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="P103" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q103" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R103" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S103" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T103" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U103" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="S103" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="T103" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U103" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="V103" s="5" t="s">
         <v>35</v>
@@ -7507,49 +7741,49 @@
         <v>35</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="J104" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S104" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K104" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L104" s="5" t="s">
+      <c r="T104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U104" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R104" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S104" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T104" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="U104" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="V104" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="W104" s="5" t="s">
         <v>35</v>
@@ -7580,22 +7814,54 @@
         <v>28</v>
       </c>
       <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
-      <c r="L105" s="5"/>
-      <c r="M105" s="5"/>
-      <c r="N105" s="5"/>
-      <c r="O105" s="5"/>
-      <c r="P105" s="5"/>
-      <c r="Q105" s="5"/>
-      <c r="R105" s="5"/>
-      <c r="S105" s="5"/>
-      <c r="T105" s="5"/>
-      <c r="U105" s="5"/>
-      <c r="V105" s="5"/>
+      <c r="G105" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H105" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N105" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O105" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R105" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S105" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T105" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U105" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V105" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="W105" s="5"/>
       <c r="X105" s="5"/>
       <c r="Y105" s="5" t="s">
@@ -7621,22 +7887,54 @@
         <v>28</v>
       </c>
       <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="5"/>
-      <c r="K106" s="5"/>
-      <c r="L106" s="5"/>
-      <c r="M106" s="5"/>
-      <c r="N106" s="5"/>
-      <c r="O106" s="5"/>
-      <c r="P106" s="5"/>
-      <c r="Q106" s="5"/>
-      <c r="R106" s="5"/>
-      <c r="S106" s="5"/>
-      <c r="T106" s="5"/>
-      <c r="U106" s="5"/>
-      <c r="V106" s="5"/>
+      <c r="G106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q106" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S106" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U106" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V106" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="W106" s="5"/>
       <c r="X106" s="5"/>
       <c r="Y106" s="5" t="s">
@@ -7668,7 +7966,7 @@
         <v>35</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I107" s="5" t="s">
         <v>30</v>
@@ -7680,13 +7978,13 @@
         <v>30</v>
       </c>
       <c r="L107" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M107" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N107" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O107" s="5" t="s">
         <v>30</v>
@@ -7695,19 +7993,19 @@
         <v>30</v>
       </c>
       <c r="Q107" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R107" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S107" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T107" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U107" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="V107" s="5" t="s">
         <v>35</v>
@@ -7747,7 +8045,7 @@
         <v>35</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I108" s="5" t="s">
         <v>30</v>
@@ -7759,13 +8057,13 @@
         <v>30</v>
       </c>
       <c r="L108" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M108" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N108" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O108" s="5" t="s">
         <v>30</v>
@@ -7777,16 +8075,16 @@
         <v>30</v>
       </c>
       <c r="R108" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="S108" s="5" t="s">
         <v>30</v>
       </c>
       <c r="T108" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U108" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="V108" s="5" t="s">
         <v>35</v>
@@ -7826,7 +8124,7 @@
         <v>35</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I109" s="5" t="s">
         <v>30</v>
@@ -7838,13 +8136,13 @@
         <v>30</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M109" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N109" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O109" s="5" t="s">
         <v>30</v>
@@ -7856,16 +8154,16 @@
         <v>30</v>
       </c>
       <c r="R109" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S109" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="T109" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U109" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V109" s="5" t="s">
         <v>35</v>
@@ -7905,10 +8203,10 @@
         <v>35</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J110" s="5" t="s">
         <v>30</v>
@@ -7917,13 +8215,13 @@
         <v>30</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M110" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N110" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O110" s="5" t="s">
         <v>30</v>
@@ -7984,7 +8282,7 @@
         <v>35</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>30</v>
@@ -7996,13 +8294,13 @@
         <v>30</v>
       </c>
       <c r="L111" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M111" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N111" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="O111" s="5" t="s">
         <v>30</v>
@@ -8063,7 +8361,7 @@
         <v>35</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I112" s="5" t="s">
         <v>30</v>
@@ -8075,13 +8373,13 @@
         <v>30</v>
       </c>
       <c r="L112" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M112" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N112" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O112" s="5" t="s">
         <v>30</v>
@@ -8142,10 +8440,10 @@
         <v>35</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J113" s="5" t="s">
         <v>30</v>
@@ -8157,10 +8455,10 @@
         <v>30</v>
       </c>
       <c r="M113" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N113" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="O113" s="5" t="s">
         <v>30</v>
@@ -8217,57 +8515,23 @@
       <c r="F114" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G114" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M114" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N114" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U114" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="V114" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W114" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="5"/>
+      <c r="O114" s="5"/>
+      <c r="P114" s="5"/>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="5"/>
+      <c r="T114" s="5"/>
+      <c r="U114" s="5"/>
+      <c r="V114" s="5"/>
+      <c r="W114" s="5"/>
       <c r="X114" s="5" t="s">
         <v>28</v>
       </c>
@@ -8764,34 +9028,34 @@
         <v>36</v>
       </c>
       <c r="N125" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O125" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P125" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q125" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R125" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S125" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T125" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O125" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P125" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q125" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R125" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="S125" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T125" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="U125" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="V125" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="W125" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="X125" s="5" t="s">
         <v>28</v>
@@ -8843,10 +9107,10 @@
         <v>32</v>
       </c>
       <c r="N126" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O126" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="P126" s="5" t="s">
         <v>30</v>
@@ -8864,13 +9128,13 @@
         <v>30</v>
       </c>
       <c r="U126" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="V126" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W126" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X126" s="5" t="s">
         <v>28</v>
@@ -8922,10 +9186,10 @@
         <v>40</v>
       </c>
       <c r="N127" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O127" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="P127" s="5" t="s">
         <v>30</v>
@@ -8934,22 +9198,22 @@
         <v>30</v>
       </c>
       <c r="R127" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S127" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T127" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U127" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V127" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W127" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X127" s="5" t="s">
         <v>28</v>
@@ -9001,34 +9265,34 @@
         <v>31</v>
       </c>
       <c r="N128" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O128" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P128" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="Q128" s="5" t="s">
         <v>30</v>
       </c>
       <c r="R128" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S128" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T128" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U128" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V128" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W128" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="T128" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U128" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="V128" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W128" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="X128" s="5" t="s">
         <v>28</v>
@@ -9080,16 +9344,16 @@
         <v>30</v>
       </c>
       <c r="N129" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O129" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P129" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q129" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="R129" s="5" t="s">
         <v>30</v>
@@ -9101,13 +9365,13 @@
         <v>30</v>
       </c>
       <c r="U129" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="V129" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W129" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X129" s="5" t="s">
         <v>28</v>
@@ -9159,34 +9423,34 @@
         <v>30</v>
       </c>
       <c r="N130" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O130" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P130" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q130" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R130" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S130" s="5" t="s">
         <v>30</v>
       </c>
       <c r="T130" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="U130" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V130" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W130" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X130" s="5" t="s">
         <v>28</v>
@@ -9238,34 +9502,34 @@
         <v>30</v>
       </c>
       <c r="N131" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="O131" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="P131" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q131" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R131" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S131" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="T131" s="5" t="s">
         <v>30</v>
       </c>
       <c r="U131" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="V131" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W131" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X131" s="5" t="s">
         <v>28</v>
@@ -9317,34 +9581,34 @@
         <v>30</v>
       </c>
       <c r="N132" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O132" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="P132" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="Q132" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R132" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="S132" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T132" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="U132" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="V132" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W132" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X132" s="5" t="s">
         <v>28</v>
@@ -9417,13 +9681,13 @@
         <v>30</v>
       </c>
       <c r="U133" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="V133" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W133" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X133" s="5" t="s">
         <v>28</v>
@@ -9490,19 +9754,19 @@
         <v>30</v>
       </c>
       <c r="S134" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T134" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U134" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="V134" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W134" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X134" s="5" t="s">
         <v>28</v>
@@ -9566,22 +9830,22 @@
         <v>30</v>
       </c>
       <c r="R135" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="S135" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T135" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U135" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="V135" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W135" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X135" s="5" t="s">
         <v>28</v>
@@ -9633,34 +9897,34 @@
         <v>30</v>
       </c>
       <c r="N136" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O136" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P136" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Q136" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R136" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="S136" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="T136" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="U136" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="V136" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W136" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X136" s="5" t="s">
         <v>28</v>
@@ -9712,10 +9976,10 @@
         <v>30</v>
       </c>
       <c r="N137" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O137" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P137" s="5" t="s">
         <v>30</v>
@@ -9730,16 +9994,16 @@
         <v>30</v>
       </c>
       <c r="T137" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U137" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="V137" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W137" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X137" s="5" t="s">
         <v>28</v>
@@ -9791,28 +10055,28 @@
         <v>31</v>
       </c>
       <c r="N138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S138" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T138" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U138" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="O138" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P138" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q138" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R138" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S138" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T138" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="U138" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="V138" s="5" t="s">
         <v>35</v>
@@ -9879,19 +10143,19 @@
         <v>30</v>
       </c>
       <c r="Q139" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R139" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S139" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="T139" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U139" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V139" s="5" t="s">
         <v>35</v>
@@ -9932,16 +10196,36 @@
       <c r="K140" s="5"/>
       <c r="L140" s="5"/>
       <c r="M140" s="5"/>
-      <c r="N140" s="5"/>
-      <c r="O140" s="5"/>
-      <c r="P140" s="5"/>
-      <c r="Q140" s="5"/>
-      <c r="R140" s="5"/>
-      <c r="S140" s="5"/>
-      <c r="T140" s="5"/>
-      <c r="U140" s="5"/>
-      <c r="V140" s="5"/>
-      <c r="W140" s="5"/>
+      <c r="N140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q140" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R140" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U140" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V140" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W140" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="X140" s="5"/>
       <c r="Y140" s="5" t="s">
         <v>28</v>
@@ -9973,16 +10257,36 @@
       <c r="K141" s="5"/>
       <c r="L141" s="5"/>
       <c r="M141" s="5"/>
-      <c r="N141" s="5"/>
-      <c r="O141" s="5"/>
-      <c r="P141" s="5"/>
-      <c r="Q141" s="5"/>
-      <c r="R141" s="5"/>
-      <c r="S141" s="5"/>
-      <c r="T141" s="5"/>
-      <c r="U141" s="5"/>
-      <c r="V141" s="5"/>
-      <c r="W141" s="5"/>
+      <c r="N141" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O141" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P141" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R141" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S141" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T141" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U141" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V141" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W141" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="X141" s="5"/>
       <c r="Y141" s="5" t="s">
         <v>28</v>
@@ -10040,22 +10344,22 @@
         <v>30</v>
       </c>
       <c r="Q142" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R142" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S142" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T142" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="U142" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="V142" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="W142" s="5" t="s">
         <v>35</v>
@@ -10119,25 +10423,25 @@
         <v>30</v>
       </c>
       <c r="Q143" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="R143" s="5" t="s">
         <v>30</v>
       </c>
       <c r="S143" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T143" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U143" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="V143" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W143" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="V143" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="W143" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="X143" s="5" t="s">
         <v>28</v>
@@ -10207,10 +10511,10 @@
         <v>30</v>
       </c>
       <c r="T144" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U144" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="V144" s="5" t="s">
         <v>35</v>
@@ -10268,25 +10572,25 @@
         <v>30</v>
       </c>
       <c r="N145" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O145" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P145" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="Q145" s="5" t="s">
         <v>30</v>
       </c>
       <c r="R145" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S145" s="5" t="s">
         <v>30</v>
       </c>
       <c r="T145" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U145" s="5" t="s">
         <v>35</v>
@@ -10362,13 +10666,13 @@
         <v>32</v>
       </c>
       <c r="S146" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="T146" s="5" t="s">
         <v>31</v>
       </c>
       <c r="U146" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V146" s="5" t="s">
         <v>35</v>
@@ -10438,16 +10742,16 @@
         <v>30</v>
       </c>
       <c r="R147" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S147" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T147" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U147" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V147" s="5" t="s">
         <v>35</v>
@@ -10517,16 +10821,16 @@
         <v>30</v>
       </c>
       <c r="R148" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S148" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T148" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="U148" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="V148" s="5" t="s">
         <v>35</v>
@@ -11072,6 +11376,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B44:Z44"/>
+    <mergeCell ref="A78:AA78"/>
+    <mergeCell ref="C2:Z2"/>
+    <mergeCell ref="B3:Z3"/>
+    <mergeCell ref="B5:Z5"/>
+    <mergeCell ref="A39:AA39"/>
+    <mergeCell ref="C41:Z41"/>
+    <mergeCell ref="B42:Z42"/>
     <mergeCell ref="D122:AB122"/>
     <mergeCell ref="C156:AC156"/>
     <mergeCell ref="C80:Z80"/>
@@ -11080,15 +11392,8 @@
     <mergeCell ref="C117:AC117"/>
     <mergeCell ref="E119:AB119"/>
     <mergeCell ref="D120:AB120"/>
-    <mergeCell ref="B44:Z44"/>
-    <mergeCell ref="A78:AA78"/>
-    <mergeCell ref="C2:Z2"/>
-    <mergeCell ref="B3:Z3"/>
-    <mergeCell ref="B5:Z5"/>
-    <mergeCell ref="A39:AA39"/>
-    <mergeCell ref="C41:Z41"/>
-    <mergeCell ref="B42:Z42"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>